<commit_message>
Added 'readme.md' document to 'docs' folder
</commit_message>
<xml_diff>
--- a/docs/project2_tennis_pt_app.xlsx
+++ b/docs/project2_tennis_pt_app.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="26680" windowHeight="17460" tabRatio="796" activeTab="1"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="28720" windowHeight="17460" tabRatio="796" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PlayerMatch_model" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="315">
   <si>
     <t>first_name</t>
   </si>
@@ -2107,9 +2107,6 @@
     <t>player_id</t>
   </si>
   <si>
-    <t>MAPPING TABLE</t>
-  </si>
-  <si>
     <t>LOCATIONS</t>
   </si>
   <si>
@@ -2272,10 +2269,10 @@
     <t>Roster Limit</t>
   </si>
   <si>
-    <t xml:space="preserve">Inherits </t>
-  </si>
-  <si>
-    <t>Attributes?</t>
+    <t>PLAYERMATCHES</t>
+  </si>
+  <si>
+    <t>playermatches_id</t>
   </si>
 </sst>
 </file>
@@ -2666,7 +2663,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2748,12 +2745,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3102,7 +3093,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="380">
+  <cellStyleXfs count="410">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3483,8 +3474,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3984,6 +4005,9 @@
     <xf numFmtId="0" fontId="59" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4005,6 +4029,36 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="56" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4023,15 +4077,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="58" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4041,15 +4086,6 @@
     <xf numFmtId="0" fontId="58" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -4065,26 +4101,38 @@
     <xf numFmtId="0" fontId="41" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="58" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="64" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="64" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="62" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="55" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="380">
+  <cellStyles count="410">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4286,6 +4334,21 @@
     <cellStyle name="Followed Hyperlink" xfId="375" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="377" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="379" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="381" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4464,6 +4527,21 @@
     <cellStyle name="Hyperlink" xfId="374" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="376" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="378" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="380" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="382" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="384" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="402" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="404" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="406" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="408" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5024,7 +5102,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="9" customFormat="1" hidden="1">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>115</v>
       </c>
       <c r="B1" s="10"/>
@@ -5077,7 +5155,7 @@
       <c r="AI1" s="11"/>
     </row>
     <row r="2" spans="1:35" s="9" customFormat="1" hidden="1">
-      <c r="A2" s="176"/>
+      <c r="A2" s="177"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -5128,7 +5206,7 @@
       <c r="AI2" s="13"/>
     </row>
     <row r="3" spans="1:35" s="9" customFormat="1" hidden="1">
-      <c r="A3" s="176"/>
+      <c r="A3" s="177"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -5175,7 +5253,7 @@
       <c r="AI3" s="13"/>
     </row>
     <row r="4" spans="1:35" s="9" customFormat="1" hidden="1">
-      <c r="A4" s="176"/>
+      <c r="A4" s="177"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -5218,7 +5296,7 @@
       <c r="AI4" s="13"/>
     </row>
     <row r="5" spans="1:35" s="9" customFormat="1" hidden="1">
-      <c r="A5" s="176"/>
+      <c r="A5" s="177"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -5257,7 +5335,7 @@
       <c r="AI5" s="13"/>
     </row>
     <row r="6" spans="1:35" s="9" customFormat="1" hidden="1">
-      <c r="A6" s="176"/>
+      <c r="A6" s="177"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -5296,7 +5374,7 @@
       <c r="AI6" s="13"/>
     </row>
     <row r="7" spans="1:35" s="9" customFormat="1" hidden="1">
-      <c r="A7" s="176"/>
+      <c r="A7" s="177"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -5382,33 +5460,33 @@
       <c r="B9" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="C9" s="179" t="str">
+      <c r="C9" s="180" t="str">
         <f>CONCATENATE(B9,B18,B17,C18,C17,D18,D17,E18,E17,F18,F17,G18,G17,H18,H17,I18,I17,J18,J17,K18,K17,L18,L17,M18,M17,N18,N17,O18,O17,P18,P17,Q18,Q17,R18,R17,S18,S17,T18,T17,U18,U17,V18,V17,W18,W17,X18,X17)</f>
         <v xml:space="preserve">rails g scaffold Player first_name:string last_name:string user_name:string password:string photo:string team_name:string role:string gender:string age_category:string skill_level:string record_ind:integer record_team:integer phone_num:string phone_type:string email:string day_pref1:string time_pref1:string day_pref2:string time_pref2:string password_digest:string remember_token:string created_at:datetime updated_at:datetime </v>
       </c>
-      <c r="D9" s="180"/>
-      <c r="E9" s="180"/>
-      <c r="F9" s="180"/>
-      <c r="G9" s="180"/>
-      <c r="H9" s="180"/>
-      <c r="I9" s="180"/>
-      <c r="J9" s="180"/>
-      <c r="K9" s="180"/>
-      <c r="L9" s="180"/>
-      <c r="M9" s="180"/>
-      <c r="N9" s="180"/>
-      <c r="O9" s="180"/>
-      <c r="P9" s="180"/>
-      <c r="Q9" s="180"/>
-      <c r="R9" s="180"/>
-      <c r="S9" s="180"/>
-      <c r="T9" s="180"/>
-      <c r="U9" s="180"/>
-      <c r="V9" s="180"/>
-      <c r="W9" s="180"/>
-      <c r="X9" s="180"/>
-      <c r="Y9" s="180"/>
-      <c r="Z9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="181"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="181"/>
+      <c r="J9" s="181"/>
+      <c r="K9" s="181"/>
+      <c r="L9" s="181"/>
+      <c r="M9" s="181"/>
+      <c r="N9" s="181"/>
+      <c r="O9" s="181"/>
+      <c r="P9" s="181"/>
+      <c r="Q9" s="181"/>
+      <c r="R9" s="181"/>
+      <c r="S9" s="181"/>
+      <c r="T9" s="181"/>
+      <c r="U9" s="181"/>
+      <c r="V9" s="181"/>
+      <c r="W9" s="181"/>
+      <c r="X9" s="181"/>
+      <c r="Y9" s="181"/>
+      <c r="Z9" s="182"/>
     </row>
     <row r="10" spans="1:35" s="35" customFormat="1" ht="23" customHeight="1">
       <c r="A10" s="34" t="s">
@@ -5417,33 +5495,33 @@
       <c r="B10" s="40" t="s">
         <v>137</v>
       </c>
-      <c r="C10" s="179" t="str">
+      <c r="C10" s="180" t="str">
         <f>CONCATENATE(B10,Y18,Y17,Z18,Z17,AA18,AA17,AB18,AB17,AC18,AC17,AD18,AD17,AE18,AE17,AF18,AF17,AG18,AG17)</f>
         <v xml:space="preserve">rails g scaffold Match match_datetime:datetime match_loc_name:string match_note:text match_opp:string match_outcome:string match_score:integer match_loc_address:string created_at:datetime updated_at:datetime </v>
       </c>
-      <c r="D10" s="180"/>
-      <c r="E10" s="180"/>
-      <c r="F10" s="180"/>
-      <c r="G10" s="180"/>
-      <c r="H10" s="180"/>
-      <c r="I10" s="180"/>
-      <c r="J10" s="180"/>
-      <c r="K10" s="180"/>
-      <c r="L10" s="180"/>
-      <c r="M10" s="180"/>
-      <c r="N10" s="180"/>
-      <c r="O10" s="180"/>
-      <c r="P10" s="180"/>
-      <c r="Q10" s="180"/>
-      <c r="R10" s="180"/>
-      <c r="S10" s="180"/>
-      <c r="T10" s="180"/>
-      <c r="U10" s="180"/>
-      <c r="V10" s="180"/>
-      <c r="W10" s="180"/>
-      <c r="X10" s="180"/>
-      <c r="Y10" s="180"/>
-      <c r="Z10" s="181"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="181"/>
+      <c r="G10" s="181"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="181"/>
+      <c r="K10" s="181"/>
+      <c r="L10" s="181"/>
+      <c r="M10" s="181"/>
+      <c r="N10" s="181"/>
+      <c r="O10" s="181"/>
+      <c r="P10" s="181"/>
+      <c r="Q10" s="181"/>
+      <c r="R10" s="181"/>
+      <c r="S10" s="181"/>
+      <c r="T10" s="181"/>
+      <c r="U10" s="181"/>
+      <c r="V10" s="181"/>
+      <c r="W10" s="181"/>
+      <c r="X10" s="181"/>
+      <c r="Y10" s="181"/>
+      <c r="Z10" s="182"/>
     </row>
     <row r="11" spans="1:35" s="35" customFormat="1" ht="23" customHeight="1">
       <c r="A11" s="36" t="s">
@@ -5452,32 +5530,32 @@
       <c r="B11" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="179" t="s">
+      <c r="C11" s="180" t="s">
         <v>139</v>
       </c>
-      <c r="D11" s="180"/>
-      <c r="E11" s="180"/>
-      <c r="F11" s="180"/>
-      <c r="G11" s="180"/>
-      <c r="H11" s="180"/>
-      <c r="I11" s="180"/>
-      <c r="J11" s="180"/>
-      <c r="K11" s="180"/>
-      <c r="L11" s="180"/>
-      <c r="M11" s="180"/>
-      <c r="N11" s="180"/>
-      <c r="O11" s="180"/>
-      <c r="P11" s="180"/>
-      <c r="Q11" s="180"/>
-      <c r="R11" s="180"/>
-      <c r="S11" s="180"/>
-      <c r="T11" s="180"/>
-      <c r="U11" s="180"/>
-      <c r="V11" s="180"/>
-      <c r="W11" s="180"/>
-      <c r="X11" s="180"/>
-      <c r="Y11" s="180"/>
-      <c r="Z11" s="181"/>
+      <c r="D11" s="181"/>
+      <c r="E11" s="181"/>
+      <c r="F11" s="181"/>
+      <c r="G11" s="181"/>
+      <c r="H11" s="181"/>
+      <c r="I11" s="181"/>
+      <c r="J11" s="181"/>
+      <c r="K11" s="181"/>
+      <c r="L11" s="181"/>
+      <c r="M11" s="181"/>
+      <c r="N11" s="181"/>
+      <c r="O11" s="181"/>
+      <c r="P11" s="181"/>
+      <c r="Q11" s="181"/>
+      <c r="R11" s="181"/>
+      <c r="S11" s="181"/>
+      <c r="T11" s="181"/>
+      <c r="U11" s="181"/>
+      <c r="V11" s="181"/>
+      <c r="W11" s="181"/>
+      <c r="X11" s="181"/>
+      <c r="Y11" s="181"/>
+      <c r="Z11" s="182"/>
     </row>
     <row r="12" spans="1:35" s="4" customFormat="1" ht="17" customHeight="1">
       <c r="A12" s="21" t="s">
@@ -6167,7 +6245,7 @@
       <c r="AI18" s="123"/>
     </row>
     <row r="19" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A19" s="177" t="s">
+      <c r="A19" s="178" t="s">
         <v>130</v>
       </c>
       <c r="B19" s="116" t="s">
@@ -6242,7 +6320,7 @@
       <c r="AI19" s="116"/>
     </row>
     <row r="20" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A20" s="178"/>
+      <c r="A20" s="179"/>
       <c r="B20" s="116" t="s">
         <v>40</v>
       </c>
@@ -6315,7 +6393,7 @@
       <c r="AI20" s="116"/>
     </row>
     <row r="21" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A21" s="178"/>
+      <c r="A21" s="179"/>
       <c r="B21" s="116" t="s">
         <v>41</v>
       </c>
@@ -6388,7 +6466,7 @@
       <c r="AI21" s="116"/>
     </row>
     <row r="22" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A22" s="178"/>
+      <c r="A22" s="179"/>
       <c r="B22" s="116" t="s">
         <v>42</v>
       </c>
@@ -6461,7 +6539,7 @@
       <c r="AI22" s="116"/>
     </row>
     <row r="23" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A23" s="178"/>
+      <c r="A23" s="179"/>
       <c r="B23" s="116" t="s">
         <v>39</v>
       </c>
@@ -6534,7 +6612,7 @@
       <c r="AI23" s="116"/>
     </row>
     <row r="24" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A24" s="178"/>
+      <c r="A24" s="179"/>
       <c r="B24" s="116" t="s">
         <v>43</v>
       </c>
@@ -6607,12 +6685,12 @@
       <c r="AI24" s="116"/>
     </row>
     <row r="25" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A25" s="178"/>
+      <c r="A25" s="179"/>
       <c r="B25" s="116" t="s">
         <v>44</v>
       </c>
       <c r="C25" s="116" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D25" s="117" t="str">
         <f t="shared" si="0"/>
@@ -6680,7 +6758,7 @@
       <c r="AI25" s="116"/>
     </row>
     <row r="26" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A26" s="178"/>
+      <c r="A26" s="179"/>
       <c r="B26" s="116" t="s">
         <v>45</v>
       </c>
@@ -6753,7 +6831,7 @@
       <c r="AI26" s="116"/>
     </row>
     <row r="27" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A27" s="178"/>
+      <c r="A27" s="179"/>
       <c r="B27" s="116" t="s">
         <v>46</v>
       </c>
@@ -6826,7 +6904,7 @@
       <c r="AI27" s="116"/>
     </row>
     <row r="28" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A28" s="178"/>
+      <c r="A28" s="179"/>
       <c r="B28" s="116" t="s">
         <v>47</v>
       </c>
@@ -6899,7 +6977,7 @@
       <c r="AI28" s="116"/>
     </row>
     <row r="29" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A29" s="178"/>
+      <c r="A29" s="179"/>
       <c r="B29" s="116" t="s">
         <v>48</v>
       </c>
@@ -6972,7 +7050,7 @@
       <c r="AI29" s="116"/>
     </row>
     <row r="30" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A30" s="178"/>
+      <c r="A30" s="179"/>
       <c r="B30" s="116" t="s">
         <v>49</v>
       </c>
@@ -7045,7 +7123,7 @@
       <c r="AI30" s="116"/>
     </row>
     <row r="31" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A31" s="178"/>
+      <c r="A31" s="179"/>
       <c r="B31" s="116" t="s">
         <v>50</v>
       </c>
@@ -7118,7 +7196,7 @@
       <c r="AI31" s="116"/>
     </row>
     <row r="32" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A32" s="178"/>
+      <c r="A32" s="179"/>
       <c r="B32" s="116" t="s">
         <v>51</v>
       </c>
@@ -7191,7 +7269,7 @@
       <c r="AI32" s="116"/>
     </row>
     <row r="33" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A33" s="178"/>
+      <c r="A33" s="179"/>
       <c r="B33" s="116" t="s">
         <v>52</v>
       </c>
@@ -7264,7 +7342,7 @@
       <c r="AI33" s="116"/>
     </row>
     <row r="34" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A34" s="178"/>
+      <c r="A34" s="179"/>
       <c r="B34" s="116" t="s">
         <v>53</v>
       </c>
@@ -7337,7 +7415,7 @@
       <c r="AI34" s="116"/>
     </row>
     <row r="35" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A35" s="178"/>
+      <c r="A35" s="179"/>
       <c r="B35" s="116" t="s">
         <v>54</v>
       </c>
@@ -7410,7 +7488,7 @@
       <c r="AI35" s="116"/>
     </row>
     <row r="36" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A36" s="178"/>
+      <c r="A36" s="179"/>
       <c r="B36" s="116" t="s">
         <v>55</v>
       </c>
@@ -7483,7 +7561,7 @@
       <c r="AI36" s="116"/>
     </row>
     <row r="37" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A37" s="178"/>
+      <c r="A37" s="179"/>
       <c r="B37" s="116" t="s">
         <v>56</v>
       </c>
@@ -7556,7 +7634,7 @@
       <c r="AI37" s="116"/>
     </row>
     <row r="38" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A38" s="178"/>
+      <c r="A38" s="179"/>
       <c r="B38" s="116" t="s">
         <v>50</v>
       </c>
@@ -7629,7 +7707,7 @@
       <c r="AI38" s="116"/>
     </row>
     <row r="39" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A39" s="178"/>
+      <c r="A39" s="179"/>
       <c r="B39" s="116" t="s">
         <v>40</v>
       </c>
@@ -7702,7 +7780,7 @@
       <c r="AI39" s="116"/>
     </row>
     <row r="40" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A40" s="178"/>
+      <c r="A40" s="179"/>
       <c r="B40" s="116" t="s">
         <v>51</v>
       </c>
@@ -7775,7 +7853,7 @@
       <c r="AI40" s="116"/>
     </row>
     <row r="41" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A41" s="178"/>
+      <c r="A41" s="179"/>
       <c r="B41" s="116" t="s">
         <v>58</v>
       </c>
@@ -7848,7 +7926,7 @@
       <c r="AI41" s="116"/>
     </row>
     <row r="42" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A42" s="178"/>
+      <c r="A42" s="179"/>
       <c r="B42" s="116" t="s">
         <v>46</v>
       </c>
@@ -7921,7 +7999,7 @@
       <c r="AI42" s="116"/>
     </row>
     <row r="43" spans="1:35" s="2" customFormat="1" ht="23" customHeight="1">
-      <c r="A43" s="178"/>
+      <c r="A43" s="179"/>
       <c r="B43" s="116" t="s">
         <v>43</v>
       </c>
@@ -8038,7 +8116,7 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="18" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
@@ -8058,7 +8136,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="9" customFormat="1" hidden="1">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="176" t="s">
         <v>115</v>
       </c>
       <c r="B1" s="10"/>
@@ -8072,7 +8150,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="9" customFormat="1" hidden="1">
-      <c r="A2" s="176"/>
+      <c r="A2" s="177"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -8084,7 +8162,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="9" customFormat="1" hidden="1">
-      <c r="A3" s="176"/>
+      <c r="A3" s="177"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -8094,7 +8172,7 @@
       <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:13" s="9" customFormat="1" hidden="1">
-      <c r="A4" s="176"/>
+      <c r="A4" s="177"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -8104,7 +8182,7 @@
       <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:13" s="9" customFormat="1" hidden="1">
-      <c r="A5" s="176"/>
+      <c r="A5" s="177"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -8114,7 +8192,7 @@
       <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:13" s="9" customFormat="1" hidden="1">
-      <c r="A6" s="176"/>
+      <c r="A6" s="177"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
@@ -8124,7 +8202,7 @@
       <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:13" s="9" customFormat="1" hidden="1">
-      <c r="A7" s="176"/>
+      <c r="A7" s="177"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -8140,100 +8218,100 @@
       <c r="B8" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="C8" s="204"/>
-      <c r="D8" s="205"/>
-      <c r="E8" s="205"/>
-      <c r="F8" s="205"/>
-      <c r="G8" s="205"/>
-      <c r="H8" s="205"/>
-      <c r="I8" s="205"/>
-      <c r="J8" s="205"/>
-      <c r="K8" s="205"/>
-      <c r="L8" s="205"/>
-      <c r="M8" s="205"/>
+      <c r="C8" s="185"/>
+      <c r="D8" s="186"/>
+      <c r="E8" s="186"/>
+      <c r="F8" s="186"/>
+      <c r="G8" s="186"/>
+      <c r="H8" s="186"/>
+      <c r="I8" s="186"/>
+      <c r="J8" s="186"/>
+      <c r="K8" s="186"/>
+      <c r="L8" s="186"/>
+      <c r="M8" s="186"/>
     </row>
     <row r="9" spans="1:13" s="35" customFormat="1" ht="23" customHeight="1">
       <c r="A9" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="B9" s="40" t="s">
         <v>304</v>
       </c>
-      <c r="B9" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="C9" s="202" t="str">
+      <c r="C9" s="183" t="str">
         <f>CONCATENATE(B9,B18,B17,C18,C17,D18,D17,E18,E17,F18,F17,G18,G17,H18,H17)</f>
         <v xml:space="preserve">rails g scaffold Group group_name:string season:string year:string gender:string skill_level:string age_category:string roster_max:integer </v>
       </c>
-      <c r="D9" s="203"/>
-      <c r="E9" s="203"/>
-      <c r="F9" s="203"/>
-      <c r="G9" s="203"/>
-      <c r="H9" s="203"/>
-      <c r="I9" s="203"/>
-      <c r="J9" s="203"/>
-      <c r="K9" s="203"/>
-      <c r="L9" s="203"/>
-      <c r="M9" s="203"/>
+      <c r="D9" s="184"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="184"/>
+      <c r="H9" s="184"/>
+      <c r="I9" s="184"/>
+      <c r="J9" s="184"/>
+      <c r="K9" s="184"/>
+      <c r="L9" s="184"/>
+      <c r="M9" s="184"/>
     </row>
     <row r="10" spans="1:13" s="35" customFormat="1" ht="23" customHeight="1">
       <c r="A10" s="34"/>
       <c r="B10" s="40"/>
-      <c r="C10" s="202"/>
-      <c r="D10" s="203"/>
-      <c r="E10" s="203"/>
-      <c r="F10" s="203"/>
-      <c r="G10" s="203"/>
-      <c r="H10" s="203"/>
-      <c r="I10" s="203"/>
-      <c r="J10" s="203"/>
-      <c r="K10" s="203"/>
-      <c r="L10" s="203"/>
-      <c r="M10" s="203"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="184"/>
+      <c r="H10" s="184"/>
+      <c r="I10" s="184"/>
+      <c r="J10" s="184"/>
+      <c r="K10" s="184"/>
+      <c r="L10" s="184"/>
+      <c r="M10" s="184"/>
     </row>
     <row r="11" spans="1:13" s="35" customFormat="1" ht="23" customHeight="1">
       <c r="A11" s="36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B11" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="202" t="s">
-        <v>308</v>
-      </c>
-      <c r="D11" s="203"/>
-      <c r="E11" s="203"/>
-      <c r="F11" s="203"/>
-      <c r="G11" s="203"/>
-      <c r="H11" s="203"/>
-      <c r="I11" s="203"/>
-      <c r="J11" s="203"/>
-      <c r="K11" s="203"/>
-      <c r="L11" s="203"/>
-      <c r="M11" s="203"/>
+      <c r="C11" s="183" t="s">
+        <v>307</v>
+      </c>
+      <c r="D11" s="184"/>
+      <c r="E11" s="184"/>
+      <c r="F11" s="184"/>
+      <c r="G11" s="184"/>
+      <c r="H11" s="184"/>
+      <c r="I11" s="184"/>
+      <c r="J11" s="184"/>
+      <c r="K11" s="184"/>
+      <c r="L11" s="184"/>
+      <c r="M11" s="184"/>
     </row>
     <row r="12" spans="1:13" s="4" customFormat="1" ht="17" customHeight="1">
       <c r="A12" s="21" t="s">
         <v>128</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" hidden="1">
@@ -8289,25 +8367,25 @@
         <v>78</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C15" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="D15" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="E15" s="16" t="s">
         <v>310</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>311</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>87</v>
       </c>
       <c r="G15" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="H15" s="16" t="s">
         <v>312</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="17" customHeight="1">
@@ -8367,13 +8445,13 @@
         <v>77</v>
       </c>
       <c r="B18" s="113" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C18" s="113" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D18" s="113" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E18" s="113" t="s">
         <v>5</v>
@@ -8385,52 +8463,52 @@
         <v>61</v>
       </c>
       <c r="H18" s="113" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="C25" s="188" t="s">
-        <v>291</v>
-      </c>
-      <c r="D25" s="189"/>
-      <c r="E25" s="190"/>
+      <c r="C25" s="187" t="s">
+        <v>290</v>
+      </c>
+      <c r="D25" s="188"/>
+      <c r="E25" s="189"/>
     </row>
     <row r="26" spans="1:8">
       <c r="C26" s="141" t="s">
         <v>221</v>
       </c>
       <c r="D26" s="142" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E26" s="142" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="C27" s="173"/>
       <c r="D27" s="174" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E27" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="C28" s="146"/>
       <c r="D28" s="147" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E28" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="C29" s="146"/>
       <c r="D29" s="147" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E29" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -8439,7 +8517,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -8448,7 +8526,7 @@
         <v>64</v>
       </c>
       <c r="E31" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -8457,34 +8535,34 @@
         <v>61</v>
       </c>
       <c r="E32" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="3:5">
       <c r="C33" s="146"/>
       <c r="D33" s="147" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E33" s="147" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="34" spans="3:5">
       <c r="C34" s="146"/>
       <c r="D34" s="147" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E34" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="3:5">
       <c r="C35" s="146"/>
       <c r="D35" s="147" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E35" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="3:5">
@@ -8492,10 +8570,10 @@
         <v>222</v>
       </c>
       <c r="D36" s="164" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E36" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37" spans="3:5">
@@ -8503,10 +8581,10 @@
         <v>222</v>
       </c>
       <c r="D37" s="164" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E37" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="38" spans="3:5">
@@ -8517,7 +8595,7 @@
         <v>258</v>
       </c>
       <c r="E38" s="166" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="39" spans="3:5">
@@ -8525,10 +8603,10 @@
         <v>222</v>
       </c>
       <c r="D39" s="166" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E39" s="166" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" spans="3:5">
@@ -8536,20 +8614,20 @@
         <v>222</v>
       </c>
       <c r="D40" s="164" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E40" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C25:E25"/>
     <mergeCell ref="A1:A7"/>
     <mergeCell ref="C9:M9"/>
     <mergeCell ref="C8:M8"/>
     <mergeCell ref="C11:M11"/>
     <mergeCell ref="C10:M10"/>
-    <mergeCell ref="C25:E25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -8568,8 +8646,8 @@
   </sheetPr>
   <dimension ref="B1:Q43"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8580,7 +8658,7 @@
     <col min="4" max="4" width="12.5" style="97" customWidth="1"/>
     <col min="5" max="5" width="13.5" style="97" customWidth="1"/>
     <col min="6" max="6" width="3.33203125" style="97" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="103" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" style="103" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5" style="135" customWidth="1"/>
     <col min="9" max="9" width="13.5" style="97" customWidth="1"/>
     <col min="10" max="10" width="3.33203125" style="97" bestFit="1" customWidth="1"/>
@@ -8600,26 +8678,26 @@
       <c r="P1" s="97"/>
     </row>
     <row r="2" spans="2:16" ht="21" customHeight="1">
-      <c r="B2" s="182" t="s">
+      <c r="B2" s="193" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="183"/>
-      <c r="D2" s="184"/>
-      <c r="F2" s="185" t="s">
-        <v>259</v>
-      </c>
-      <c r="G2" s="186"/>
-      <c r="H2" s="187"/>
-      <c r="J2" s="191" t="s">
-        <v>266</v>
-      </c>
-      <c r="K2" s="192"/>
-      <c r="L2" s="193"/>
-      <c r="N2" s="194" t="s">
+      <c r="C2" s="194"/>
+      <c r="D2" s="195"/>
+      <c r="F2" s="196" t="s">
+        <v>313</v>
+      </c>
+      <c r="G2" s="197"/>
+      <c r="H2" s="198"/>
+      <c r="J2" s="199" t="s">
+        <v>265</v>
+      </c>
+      <c r="K2" s="200"/>
+      <c r="L2" s="201"/>
+      <c r="N2" s="190" t="s">
         <v>219</v>
       </c>
-      <c r="O2" s="195"/>
-      <c r="P2" s="196"/>
+      <c r="O2" s="191"/>
+      <c r="P2" s="192"/>
     </row>
     <row r="3" spans="2:16">
       <c r="B3" s="137" t="s">
@@ -8629,25 +8707,25 @@
         <v>257</v>
       </c>
       <c r="D3" s="138" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F3" s="102" t="s">
         <v>221</v>
       </c>
       <c r="G3" s="100" t="s">
-        <v>262</v>
+        <v>314</v>
       </c>
       <c r="H3" s="100" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J3" s="139" t="s">
         <v>221</v>
       </c>
       <c r="K3" s="140" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L3" s="140" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="N3" s="169" t="s">
         <v>221</v>
@@ -8656,7 +8734,7 @@
         <v>258</v>
       </c>
       <c r="P3" s="170" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="2:16">
@@ -8665,30 +8743,28 @@
         <v>116</v>
       </c>
       <c r="D4" s="136" t="s">
-        <v>269</v>
-      </c>
-      <c r="F4" s="143" t="s">
-        <v>222</v>
-      </c>
-      <c r="G4" s="144" t="s">
-        <v>286</v>
-      </c>
-      <c r="H4" s="144" t="s">
-        <v>272</v>
+        <v>268</v>
+      </c>
+      <c r="F4" s="215"/>
+      <c r="G4" s="216" t="s">
+        <v>247</v>
+      </c>
+      <c r="H4" s="216" t="s">
+        <v>268</v>
       </c>
       <c r="J4" s="143"/>
       <c r="K4" s="144" t="s">
         <v>2</v>
       </c>
       <c r="L4" s="144" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N4" s="171"/>
       <c r="O4" s="172" t="s">
         <v>0</v>
       </c>
       <c r="P4" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="2:16">
@@ -8697,30 +8773,28 @@
         <v>118</v>
       </c>
       <c r="D5" s="136" t="s">
-        <v>267</v>
-      </c>
-      <c r="F5" s="145" t="s">
-        <v>222</v>
-      </c>
-      <c r="G5" s="136" t="s">
-        <v>257</v>
-      </c>
-      <c r="H5" s="136" t="s">
-        <v>272</v>
+        <v>266</v>
+      </c>
+      <c r="F5" s="215"/>
+      <c r="G5" s="216" t="s">
+        <v>248</v>
+      </c>
+      <c r="H5" s="216" t="s">
+        <v>268</v>
       </c>
       <c r="J5" s="143"/>
       <c r="K5" s="144" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L5" s="144" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N5" s="171"/>
       <c r="O5" s="172" t="s">
         <v>1</v>
       </c>
       <c r="P5" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6" spans="2:16">
@@ -8729,30 +8803,30 @@
         <v>123</v>
       </c>
       <c r="D6" s="136" t="s">
-        <v>284</v>
-      </c>
-      <c r="F6" s="146" t="s">
+        <v>283</v>
+      </c>
+      <c r="F6" s="207" t="s">
         <v>222</v>
       </c>
-      <c r="G6" s="147" t="s">
-        <v>300</v>
-      </c>
-      <c r="H6" s="147" t="s">
-        <v>272</v>
+      <c r="G6" s="208" t="s">
+        <v>285</v>
+      </c>
+      <c r="H6" s="208" t="s">
+        <v>271</v>
       </c>
       <c r="J6" s="143"/>
       <c r="K6" s="144" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L6" s="144" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N6" s="171"/>
       <c r="O6" s="172" t="s">
         <v>11</v>
       </c>
       <c r="P6" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="2:16">
@@ -8761,30 +8835,30 @@
         <v>120</v>
       </c>
       <c r="D7" s="136" t="s">
-        <v>267</v>
-      </c>
-      <c r="F7" s="148" t="s">
+        <v>266</v>
+      </c>
+      <c r="F7" s="209" t="s">
         <v>222</v>
       </c>
-      <c r="G7" s="149" t="s">
-        <v>261</v>
-      </c>
-      <c r="H7" s="149" t="s">
-        <v>272</v>
+      <c r="G7" s="210" t="s">
+        <v>257</v>
+      </c>
+      <c r="H7" s="210" t="s">
+        <v>271</v>
       </c>
       <c r="J7" s="143"/>
       <c r="K7" s="144" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L7" s="144" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N7" s="171"/>
       <c r="O7" s="172" t="s">
         <v>63</v>
       </c>
       <c r="P7" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="2:16">
@@ -8793,33 +8867,30 @@
         <v>65</v>
       </c>
       <c r="D8" s="136" t="s">
-        <v>267</v>
-      </c>
-      <c r="F8" s="171" t="s">
+        <v>266</v>
+      </c>
+      <c r="F8" s="211" t="s">
         <v>222</v>
       </c>
-      <c r="G8" s="172" t="s">
+      <c r="G8" s="212" t="s">
         <v>258</v>
       </c>
-      <c r="H8" s="172" t="s">
-        <v>272</v>
+      <c r="H8" s="212" t="s">
+        <v>271</v>
       </c>
       <c r="J8" s="143"/>
       <c r="K8" s="144" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L8" s="144" t="s">
-        <v>269</v>
-      </c>
-      <c r="M8" s="207" t="s">
-        <v>314</v>
+        <v>268</v>
       </c>
       <c r="N8" s="171"/>
       <c r="O8" s="172" t="s">
         <v>107</v>
       </c>
       <c r="P8" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="2:16" s="98" customFormat="1">
@@ -8828,27 +8899,31 @@
         <v>74</v>
       </c>
       <c r="D9" s="136" t="s">
-        <v>267</v>
-      </c>
-      <c r="F9" s="101"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
+        <v>266</v>
+      </c>
+      <c r="F9" s="213" t="s">
+        <v>222</v>
+      </c>
+      <c r="G9" s="214" t="s">
+        <v>260</v>
+      </c>
+      <c r="H9" s="214" t="s">
+        <v>271</v>
+      </c>
       <c r="J9" s="143"/>
       <c r="K9" s="144" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L9" s="144" t="s">
-        <v>272</v>
-      </c>
-      <c r="M9" s="207" t="s">
-        <v>315</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="M9" s="103"/>
       <c r="N9" s="171"/>
       <c r="O9" s="172" t="s">
         <v>5</v>
       </c>
       <c r="P9" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="2:16">
@@ -8857,24 +8932,24 @@
         <v>247</v>
       </c>
       <c r="D10" s="136" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F10" s="101"/>
       <c r="G10" s="99"/>
       <c r="H10" s="99"/>
       <c r="J10" s="143"/>
       <c r="K10" s="144" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L10" s="144" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N10" s="171"/>
       <c r="O10" s="172" t="s">
         <v>61</v>
       </c>
       <c r="P10" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="2:16">
@@ -8883,68 +8958,80 @@
         <v>248</v>
       </c>
       <c r="D11" s="136" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F11" s="101"/>
       <c r="G11" s="99"/>
       <c r="H11" s="99"/>
       <c r="J11" s="143"/>
       <c r="K11" s="144" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L11" s="144" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N11" s="171"/>
       <c r="O11" s="172" t="s">
         <v>64</v>
       </c>
       <c r="P11" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="2:16">
-      <c r="B12" s="145"/>
-      <c r="C12" s="136"/>
-      <c r="D12" s="136"/>
+      <c r="B12" s="139" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="140" t="s">
+        <v>285</v>
+      </c>
+      <c r="D12" s="140" t="s">
+        <v>271</v>
+      </c>
       <c r="F12" s="101"/>
       <c r="G12" s="99"/>
       <c r="H12" s="99"/>
       <c r="J12" s="143"/>
       <c r="K12" s="144" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L12" s="144" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N12" s="171"/>
       <c r="O12" s="172" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="P12" s="172" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="2:16">
-      <c r="B13" s="145"/>
-      <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
+      <c r="B13" s="163" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" s="164" t="s">
+        <v>260</v>
+      </c>
+      <c r="D13" s="164" t="s">
+        <v>271</v>
+      </c>
       <c r="F13" s="101"/>
       <c r="G13" s="99"/>
       <c r="H13" s="99"/>
       <c r="J13" s="143"/>
       <c r="K13" s="144" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L13" s="144" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="N13" s="171"/>
       <c r="O13" s="172" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P13" s="172" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="2:16">
@@ -8952,80 +9039,80 @@
         <v>222</v>
       </c>
       <c r="C14" s="164" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D14" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E14" s="167"/>
       <c r="F14" s="163" t="s">
         <v>222</v>
       </c>
       <c r="G14" s="164" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H14" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J14" s="143"/>
       <c r="K14" s="144" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L14" s="144" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N14" s="171"/>
       <c r="O14" s="172" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="P14" s="172" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="2:16">
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="C15" s="166" t="s">
-        <v>300</v>
-      </c>
-      <c r="D15" s="166" t="s">
-        <v>272</v>
+      <c r="C15" s="164" t="s">
+        <v>299</v>
+      </c>
+      <c r="D15" s="164" t="s">
+        <v>271</v>
       </c>
       <c r="E15" s="167"/>
       <c r="F15" s="163" t="s">
         <v>222</v>
       </c>
       <c r="G15" s="164" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H15" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J15" s="143"/>
       <c r="K15" s="144" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L15" s="144" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N15" s="171"/>
       <c r="O15" s="172" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="P15" s="172" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="2:16">
-      <c r="B16" s="165" t="s">
+      <c r="B16" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="C16" s="166" t="s">
+      <c r="C16" s="164" t="s">
         <v>258</v>
       </c>
-      <c r="D16" s="166" t="s">
-        <v>272</v>
+      <c r="D16" s="164" t="s">
+        <v>271</v>
       </c>
       <c r="E16" s="167"/>
       <c r="F16" s="163" t="s">
@@ -9035,91 +9122,91 @@
         <v>258</v>
       </c>
       <c r="H16" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J16" s="143"/>
       <c r="K16" s="144" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L16" s="144" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N16" s="171"/>
       <c r="O16" s="172" t="s">
         <v>4</v>
       </c>
       <c r="P16" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="2:16">
-      <c r="B17" s="165" t="s">
+      <c r="B17" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="C17" s="166" t="s">
-        <v>286</v>
-      </c>
-      <c r="D17" s="166" t="s">
-        <v>272</v>
+      <c r="C17" s="164" t="s">
+        <v>285</v>
+      </c>
+      <c r="D17" s="164" t="s">
+        <v>271</v>
       </c>
       <c r="E17" s="167"/>
       <c r="F17" s="163" t="s">
         <v>222</v>
       </c>
       <c r="G17" s="164" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H17" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J17" s="143"/>
       <c r="K17" s="144" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L17" s="144" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="N17" s="171"/>
       <c r="O17" s="172" t="s">
         <v>3</v>
       </c>
       <c r="P17" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="2:16">
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="C18" s="166" t="s">
-        <v>262</v>
-      </c>
-      <c r="D18" s="166" t="s">
-        <v>272</v>
+      <c r="C18" s="164" t="s">
+        <v>261</v>
+      </c>
+      <c r="D18" s="164" t="s">
+        <v>271</v>
       </c>
       <c r="E18" s="167"/>
       <c r="F18" s="163" t="s">
         <v>222</v>
       </c>
       <c r="G18" s="164" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H18" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J18" s="143"/>
       <c r="K18" s="144" t="s">
         <v>247</v>
       </c>
       <c r="L18" s="144" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N18" s="171"/>
       <c r="O18" s="172" t="s">
         <v>2</v>
       </c>
       <c r="P18" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="2:16">
@@ -9128,36 +9215,36 @@
         <v>248</v>
       </c>
       <c r="L19" s="144" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="N19" s="171"/>
       <c r="O19" s="172" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P19" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="2:16">
-      <c r="B20" s="188" t="s">
-        <v>291</v>
-      </c>
-      <c r="C20" s="189"/>
-      <c r="D20" s="190"/>
-      <c r="F20" s="185" t="s">
-        <v>260</v>
-      </c>
-      <c r="G20" s="186"/>
-      <c r="H20" s="187"/>
-      <c r="J20" s="143"/>
-      <c r="K20" s="144"/>
-      <c r="L20" s="144"/>
+      <c r="B20" s="187" t="s">
+        <v>290</v>
+      </c>
+      <c r="C20" s="188"/>
+      <c r="D20" s="189"/>
+      <c r="F20" s="196" t="s">
+        <v>259</v>
+      </c>
+      <c r="G20" s="197"/>
+      <c r="H20" s="198"/>
+      <c r="J20" s="163"/>
+      <c r="K20" s="164"/>
+      <c r="L20" s="164"/>
       <c r="N20" s="171"/>
       <c r="O20" s="172" t="s">
         <v>12</v>
       </c>
       <c r="P20" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="2:16">
@@ -9165,19 +9252,19 @@
         <v>221</v>
       </c>
       <c r="C21" s="142" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D21" s="142" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F21" s="150" t="s">
         <v>221</v>
       </c>
       <c r="G21" s="151" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H21" s="151" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J21" s="143"/>
       <c r="K21" s="144"/>
@@ -9187,23 +9274,23 @@
         <v>6</v>
       </c>
       <c r="P21" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="2:16">
       <c r="B22" s="173"/>
       <c r="C22" s="174" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D22" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F22" s="148"/>
       <c r="G22" s="149" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H22" s="149" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J22" s="143"/>
       <c r="K22" s="144"/>
@@ -9213,23 +9300,23 @@
         <v>13</v>
       </c>
       <c r="P22" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="2:16">
       <c r="B23" s="146"/>
       <c r="C23" s="147" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D23" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F23" s="148"/>
       <c r="G23" s="149" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H23" s="149" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J23" s="143"/>
       <c r="K23" s="144"/>
@@ -9239,30 +9326,36 @@
         <v>7</v>
       </c>
       <c r="P23" s="172" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="2:16">
       <c r="B24" s="146"/>
       <c r="C24" s="147" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D24" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F24" s="148"/>
       <c r="G24" s="149" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H24" s="149" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J24" s="143"/>
       <c r="K24" s="144"/>
       <c r="L24" s="144"/>
-      <c r="N24" s="171"/>
-      <c r="O24" s="172"/>
-      <c r="P24" s="172"/>
+      <c r="N24" s="163" t="s">
+        <v>222</v>
+      </c>
+      <c r="O24" s="164" t="s">
+        <v>260</v>
+      </c>
+      <c r="P24" s="164" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="25" spans="2:16">
       <c r="B25" s="146"/>
@@ -9270,34 +9363,25 @@
         <v>5</v>
       </c>
       <c r="D25" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F25" s="148"/>
       <c r="G25" s="149" t="s">
         <v>247</v>
       </c>
       <c r="H25" s="149" t="s">
-        <v>269</v>
-      </c>
-      <c r="J25" s="165" t="s">
+        <v>268</v>
+      </c>
+      <c r="J25" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="K25" s="166" t="s">
-        <v>261</v>
-      </c>
-      <c r="L25" s="166" t="s">
-        <v>272</v>
-      </c>
-      <c r="M25" s="206"/>
-      <c r="N25" s="165" t="s">
-        <v>222</v>
-      </c>
-      <c r="O25" s="166" t="s">
-        <v>261</v>
-      </c>
-      <c r="P25" s="166" t="s">
-        <v>272</v>
-      </c>
+      <c r="K25" s="164" t="s">
+        <v>260</v>
+      </c>
+      <c r="L25" s="164" t="s">
+        <v>271</v>
+      </c>
+      <c r="M25" s="175"/>
     </row>
     <row r="26" spans="2:16">
       <c r="B26" s="146"/>
@@ -9305,33 +9389,33 @@
         <v>64</v>
       </c>
       <c r="D26" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F26" s="148"/>
       <c r="G26" s="149" t="s">
         <v>248</v>
       </c>
       <c r="H26" s="149" t="s">
-        <v>269</v>
-      </c>
-      <c r="J26" s="165" t="s">
+        <v>268</v>
+      </c>
+      <c r="J26" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="K26" s="166" t="s">
-        <v>300</v>
-      </c>
-      <c r="L26" s="166" t="s">
-        <v>272</v>
-      </c>
-      <c r="M26" s="206"/>
-      <c r="N26" s="165" t="s">
+      <c r="K26" s="164" t="s">
+        <v>299</v>
+      </c>
+      <c r="L26" s="164" t="s">
+        <v>271</v>
+      </c>
+      <c r="M26" s="175"/>
+      <c r="N26" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="O26" s="166" t="s">
-        <v>300</v>
-      </c>
-      <c r="P26" s="166" t="s">
-        <v>272</v>
+      <c r="O26" s="164" t="s">
+        <v>299</v>
+      </c>
+      <c r="P26" s="164" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="27" spans="2:16">
@@ -9340,21 +9424,21 @@
         <v>61</v>
       </c>
       <c r="D27" s="147" t="s">
-        <v>267</v>
-      </c>
-      <c r="F27" s="148"/>
-      <c r="G27" s="149"/>
-      <c r="H27" s="149"/>
-      <c r="J27" s="165" t="s">
+        <v>266</v>
+      </c>
+      <c r="F27" s="163"/>
+      <c r="G27" s="164"/>
+      <c r="H27" s="164"/>
+      <c r="J27" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="K27" s="166" t="s">
+      <c r="K27" s="164" t="s">
         <v>258</v>
       </c>
-      <c r="L27" s="166" t="s">
-        <v>272</v>
-      </c>
-      <c r="M27" s="206"/>
+      <c r="L27" s="164" t="s">
+        <v>271</v>
+      </c>
+      <c r="M27" s="175"/>
       <c r="N27" s="163" t="s">
         <v>222</v>
       </c>
@@ -9362,16 +9446,16 @@
         <v>258</v>
       </c>
       <c r="P27" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="28" spans="2:16">
       <c r="B28" s="146"/>
       <c r="C28" s="147" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D28" s="147" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F28" s="148"/>
       <c r="G28" s="149"/>
@@ -9380,94 +9464,94 @@
         <v>222</v>
       </c>
       <c r="K28" s="164" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L28" s="164" t="s">
-        <v>272</v>
-      </c>
-      <c r="M28" s="206"/>
-      <c r="N28" s="165" t="s">
+        <v>271</v>
+      </c>
+      <c r="M28" s="175"/>
+      <c r="N28" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="O28" s="166" t="s">
-        <v>286</v>
-      </c>
-      <c r="P28" s="166" t="s">
-        <v>272</v>
+      <c r="O28" s="164" t="s">
+        <v>285</v>
+      </c>
+      <c r="P28" s="164" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="29" spans="2:16">
       <c r="B29" s="146"/>
       <c r="C29" s="147" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D29" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F29" s="148"/>
       <c r="G29" s="149"/>
       <c r="H29" s="149"/>
-      <c r="J29" s="165" t="s">
+      <c r="J29" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="K29" s="166" t="s">
-        <v>262</v>
-      </c>
-      <c r="L29" s="166" t="s">
-        <v>272</v>
-      </c>
-      <c r="M29" s="206"/>
-      <c r="N29" s="165" t="s">
+      <c r="K29" s="164" t="s">
+        <v>261</v>
+      </c>
+      <c r="L29" s="164" t="s">
+        <v>271</v>
+      </c>
+      <c r="M29" s="175"/>
+      <c r="N29" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="O29" s="166" t="s">
-        <v>262</v>
-      </c>
-      <c r="P29" s="166" t="s">
-        <v>272</v>
+      <c r="O29" s="164" t="s">
+        <v>261</v>
+      </c>
+      <c r="P29" s="164" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="30" spans="2:16">
       <c r="B30" s="146"/>
       <c r="C30" s="147" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D30" s="147" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E30" s="168"/>
       <c r="F30" s="163" t="s">
         <v>222</v>
       </c>
       <c r="G30" s="164" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H30" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J30" s="158"/>
       <c r="K30" s="159"/>
       <c r="L30" s="159"/>
     </row>
     <row r="31" spans="2:16">
-      <c r="B31" s="163" t="s">
+      <c r="B31" s="139" t="s">
         <v>222</v>
       </c>
-      <c r="C31" s="164" t="s">
-        <v>261</v>
-      </c>
-      <c r="D31" s="164" t="s">
-        <v>272</v>
+      <c r="C31" s="140" t="s">
+        <v>285</v>
+      </c>
+      <c r="D31" s="140" t="s">
+        <v>271</v>
       </c>
       <c r="E31" s="168"/>
-      <c r="F31" s="165" t="s">
+      <c r="F31" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="G31" s="166" t="s">
-        <v>300</v>
-      </c>
-      <c r="H31" s="166" t="s">
-        <v>272</v>
+      <c r="G31" s="164" t="s">
+        <v>299</v>
+      </c>
+      <c r="H31" s="164" t="s">
+        <v>271</v>
       </c>
       <c r="J31" s="158"/>
       <c r="K31" s="159"/>
@@ -9478,68 +9562,68 @@
         <v>222</v>
       </c>
       <c r="C32" s="164" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D32" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E32" s="168"/>
-      <c r="F32" s="165" t="s">
+      <c r="F32" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="G32" s="166" t="s">
+      <c r="G32" s="164" t="s">
         <v>258</v>
       </c>
-      <c r="H32" s="166" t="s">
-        <v>272</v>
+      <c r="H32" s="164" t="s">
+        <v>271</v>
       </c>
       <c r="J32" s="158"/>
       <c r="K32" s="159"/>
       <c r="L32" s="159"/>
     </row>
     <row r="33" spans="2:16">
-      <c r="B33" s="165" t="s">
+      <c r="B33" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="C33" s="166" t="s">
+      <c r="C33" s="164" t="s">
         <v>258</v>
       </c>
-      <c r="D33" s="166" t="s">
-        <v>272</v>
+      <c r="D33" s="164" t="s">
+        <v>271</v>
       </c>
       <c r="E33" s="168"/>
-      <c r="F33" s="165" t="s">
+      <c r="F33" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="G33" s="166" t="s">
-        <v>286</v>
-      </c>
-      <c r="H33" s="166" t="s">
-        <v>272</v>
+      <c r="G33" s="164" t="s">
+        <v>285</v>
+      </c>
+      <c r="H33" s="164" t="s">
+        <v>271</v>
       </c>
       <c r="J33" s="158"/>
       <c r="K33" s="159"/>
       <c r="L33" s="159"/>
     </row>
     <row r="34" spans="2:16">
-      <c r="B34" s="165" t="s">
+      <c r="B34" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="C34" s="166" t="s">
-        <v>286</v>
-      </c>
-      <c r="D34" s="166" t="s">
-        <v>272</v>
+      <c r="C34" s="164" t="s">
+        <v>285</v>
+      </c>
+      <c r="D34" s="164" t="s">
+        <v>271</v>
       </c>
       <c r="E34" s="168"/>
-      <c r="F34" s="165" t="s">
+      <c r="F34" s="163" t="s">
         <v>222</v>
       </c>
-      <c r="G34" s="166" t="s">
-        <v>262</v>
-      </c>
-      <c r="H34" s="166" t="s">
-        <v>272</v>
+      <c r="G34" s="164" t="s">
+        <v>261</v>
+      </c>
+      <c r="H34" s="164" t="s">
+        <v>271</v>
       </c>
       <c r="J34" s="158"/>
       <c r="K34" s="159"/>
@@ -9550,10 +9634,10 @@
         <v>222</v>
       </c>
       <c r="C35" s="164" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D35" s="164" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J35" s="158"/>
       <c r="K35" s="159"/>
@@ -9971,22 +10055,22 @@
       <c r="B15" s="92"/>
       <c r="C15" s="92"/>
       <c r="D15" s="94"/>
-      <c r="E15" s="199" t="s">
+      <c r="E15" s="204" t="s">
         <v>141</v>
       </c>
-      <c r="F15" s="200"/>
-      <c r="G15" s="200"/>
-      <c r="H15" s="200"/>
-      <c r="I15" s="200"/>
-      <c r="J15" s="200"/>
-      <c r="K15" s="200"/>
-      <c r="L15" s="200"/>
-      <c r="M15" s="200"/>
-      <c r="N15" s="200"/>
-      <c r="O15" s="200"/>
-      <c r="P15" s="200"/>
-      <c r="Q15" s="200"/>
-      <c r="R15" s="200"/>
+      <c r="F15" s="205"/>
+      <c r="G15" s="205"/>
+      <c r="H15" s="205"/>
+      <c r="I15" s="205"/>
+      <c r="J15" s="205"/>
+      <c r="K15" s="205"/>
+      <c r="L15" s="205"/>
+      <c r="M15" s="205"/>
+      <c r="N15" s="205"/>
+      <c r="O15" s="205"/>
+      <c r="P15" s="205"/>
+      <c r="Q15" s="205"/>
+      <c r="R15" s="205"/>
     </row>
     <row r="16" spans="1:18" s="67" customFormat="1" ht="13" customHeight="1">
       <c r="A16" s="107"/>
@@ -10013,22 +10097,22 @@
       <c r="B17" s="92"/>
       <c r="C17" s="92"/>
       <c r="D17" s="94"/>
-      <c r="E17" s="199" t="s">
+      <c r="E17" s="204" t="s">
         <v>142</v>
       </c>
-      <c r="F17" s="200"/>
-      <c r="G17" s="200"/>
-      <c r="H17" s="200"/>
-      <c r="I17" s="200"/>
-      <c r="J17" s="200"/>
-      <c r="K17" s="200"/>
-      <c r="L17" s="200"/>
-      <c r="M17" s="200"/>
-      <c r="N17" s="200"/>
-      <c r="O17" s="200"/>
-      <c r="P17" s="200"/>
-      <c r="Q17" s="200"/>
-      <c r="R17" s="200"/>
+      <c r="F17" s="205"/>
+      <c r="G17" s="205"/>
+      <c r="H17" s="205"/>
+      <c r="I17" s="205"/>
+      <c r="J17" s="205"/>
+      <c r="K17" s="205"/>
+      <c r="L17" s="205"/>
+      <c r="M17" s="205"/>
+      <c r="N17" s="205"/>
+      <c r="O17" s="205"/>
+      <c r="P17" s="205"/>
+      <c r="Q17" s="205"/>
+      <c r="R17" s="205"/>
     </row>
     <row r="18" spans="1:18" s="67" customFormat="1" ht="13" customHeight="1">
       <c r="A18" s="107"/>
@@ -10055,22 +10139,22 @@
       <c r="B19" s="92"/>
       <c r="C19" s="92"/>
       <c r="D19" s="94"/>
-      <c r="E19" s="199" t="s">
+      <c r="E19" s="204" t="s">
         <v>143</v>
       </c>
-      <c r="F19" s="200"/>
-      <c r="G19" s="200"/>
-      <c r="H19" s="200"/>
-      <c r="I19" s="200"/>
-      <c r="J19" s="200"/>
-      <c r="K19" s="200"/>
-      <c r="L19" s="200"/>
-      <c r="M19" s="200"/>
-      <c r="N19" s="200"/>
-      <c r="O19" s="200"/>
-      <c r="P19" s="200"/>
-      <c r="Q19" s="200"/>
-      <c r="R19" s="200"/>
+      <c r="F19" s="205"/>
+      <c r="G19" s="205"/>
+      <c r="H19" s="205"/>
+      <c r="I19" s="205"/>
+      <c r="J19" s="205"/>
+      <c r="K19" s="205"/>
+      <c r="L19" s="205"/>
+      <c r="M19" s="205"/>
+      <c r="N19" s="205"/>
+      <c r="O19" s="205"/>
+      <c r="P19" s="205"/>
+      <c r="Q19" s="205"/>
+      <c r="R19" s="205"/>
     </row>
     <row r="20" spans="1:18" s="67" customFormat="1" ht="17" customHeight="1">
       <c r="A20" s="107"/>
@@ -10141,22 +10225,22 @@
       <c r="B23" s="92"/>
       <c r="C23" s="92"/>
       <c r="D23" s="94"/>
-      <c r="E23" s="199" t="s">
+      <c r="E23" s="204" t="s">
         <v>144</v>
       </c>
-      <c r="F23" s="200"/>
-      <c r="G23" s="200"/>
-      <c r="H23" s="200"/>
-      <c r="I23" s="200"/>
-      <c r="J23" s="200"/>
-      <c r="K23" s="200"/>
-      <c r="L23" s="200"/>
-      <c r="M23" s="200"/>
-      <c r="N23" s="200"/>
-      <c r="O23" s="200"/>
-      <c r="P23" s="200"/>
-      <c r="Q23" s="200"/>
-      <c r="R23" s="200"/>
+      <c r="F23" s="205"/>
+      <c r="G23" s="205"/>
+      <c r="H23" s="205"/>
+      <c r="I23" s="205"/>
+      <c r="J23" s="205"/>
+      <c r="K23" s="205"/>
+      <c r="L23" s="205"/>
+      <c r="M23" s="205"/>
+      <c r="N23" s="205"/>
+      <c r="O23" s="205"/>
+      <c r="P23" s="205"/>
+      <c r="Q23" s="205"/>
+      <c r="R23" s="205"/>
     </row>
     <row r="24" spans="1:18" s="67" customFormat="1" ht="17" customHeight="1">
       <c r="A24" s="107"/>
@@ -10227,22 +10311,22 @@
       <c r="B27" s="92"/>
       <c r="C27" s="92"/>
       <c r="D27" s="94"/>
-      <c r="E27" s="199" t="s">
+      <c r="E27" s="204" t="s">
         <v>145</v>
       </c>
-      <c r="F27" s="200"/>
-      <c r="G27" s="200"/>
-      <c r="H27" s="200"/>
-      <c r="I27" s="200"/>
-      <c r="J27" s="200"/>
-      <c r="K27" s="200"/>
-      <c r="L27" s="200"/>
-      <c r="M27" s="200"/>
-      <c r="N27" s="200"/>
-      <c r="O27" s="200"/>
-      <c r="P27" s="200"/>
-      <c r="Q27" s="200"/>
-      <c r="R27" s="200"/>
+      <c r="F27" s="205"/>
+      <c r="G27" s="205"/>
+      <c r="H27" s="205"/>
+      <c r="I27" s="205"/>
+      <c r="J27" s="205"/>
+      <c r="K27" s="205"/>
+      <c r="L27" s="205"/>
+      <c r="M27" s="205"/>
+      <c r="N27" s="205"/>
+      <c r="O27" s="205"/>
+      <c r="P27" s="205"/>
+      <c r="Q27" s="205"/>
+      <c r="R27" s="205"/>
     </row>
     <row r="28" spans="1:18" s="67" customFormat="1" ht="17" customHeight="1">
       <c r="A28" s="107"/>
@@ -10313,22 +10397,22 @@
       <c r="B31" s="92"/>
       <c r="C31" s="92"/>
       <c r="D31" s="94"/>
-      <c r="E31" s="199" t="s">
+      <c r="E31" s="204" t="s">
         <v>211</v>
       </c>
-      <c r="F31" s="200"/>
-      <c r="G31" s="200"/>
-      <c r="H31" s="200"/>
-      <c r="I31" s="200"/>
-      <c r="J31" s="200"/>
-      <c r="K31" s="200"/>
-      <c r="L31" s="200"/>
-      <c r="M31" s="200"/>
-      <c r="N31" s="200"/>
-      <c r="O31" s="200"/>
-      <c r="P31" s="200"/>
-      <c r="Q31" s="200"/>
-      <c r="R31" s="200"/>
+      <c r="F31" s="205"/>
+      <c r="G31" s="205"/>
+      <c r="H31" s="205"/>
+      <c r="I31" s="205"/>
+      <c r="J31" s="205"/>
+      <c r="K31" s="205"/>
+      <c r="L31" s="205"/>
+      <c r="M31" s="205"/>
+      <c r="N31" s="205"/>
+      <c r="O31" s="205"/>
+      <c r="P31" s="205"/>
+      <c r="Q31" s="205"/>
+      <c r="R31" s="205"/>
     </row>
     <row r="32" spans="1:18" s="67" customFormat="1" ht="17" customHeight="1">
       <c r="A32" s="107"/>
@@ -10463,22 +10547,22 @@
       <c r="B38" s="92"/>
       <c r="C38" s="92"/>
       <c r="D38" s="94"/>
-      <c r="E38" s="199" t="s">
+      <c r="E38" s="204" t="s">
         <v>210</v>
       </c>
-      <c r="F38" s="200"/>
-      <c r="G38" s="200"/>
-      <c r="H38" s="200"/>
-      <c r="I38" s="200"/>
-      <c r="J38" s="200"/>
-      <c r="K38" s="200"/>
-      <c r="L38" s="200"/>
-      <c r="M38" s="200"/>
-      <c r="N38" s="200"/>
-      <c r="O38" s="200"/>
-      <c r="P38" s="200"/>
-      <c r="Q38" s="200"/>
-      <c r="R38" s="200"/>
+      <c r="F38" s="205"/>
+      <c r="G38" s="205"/>
+      <c r="H38" s="205"/>
+      <c r="I38" s="205"/>
+      <c r="J38" s="205"/>
+      <c r="K38" s="205"/>
+      <c r="L38" s="205"/>
+      <c r="M38" s="205"/>
+      <c r="N38" s="205"/>
+      <c r="O38" s="205"/>
+      <c r="P38" s="205"/>
+      <c r="Q38" s="205"/>
+      <c r="R38" s="205"/>
     </row>
     <row r="39" spans="1:18" s="67" customFormat="1" ht="17" customHeight="1">
       <c r="A39" s="107"/>
@@ -10657,16 +10741,16 @@
       <c r="B47" s="92"/>
       <c r="C47" s="92"/>
       <c r="D47" s="94"/>
-      <c r="E47" s="199" t="s">
+      <c r="E47" s="204" t="s">
         <v>204</v>
       </c>
-      <c r="F47" s="201"/>
+      <c r="F47" s="206"/>
       <c r="G47" s="94"/>
-      <c r="H47" s="199" t="s">
+      <c r="H47" s="204" t="s">
         <v>205</v>
       </c>
-      <c r="I47" s="200"/>
-      <c r="J47" s="200"/>
+      <c r="I47" s="205"/>
+      <c r="J47" s="205"/>
       <c r="K47" s="92"/>
       <c r="L47" s="92"/>
       <c r="M47" s="92"/>
@@ -10874,22 +10958,22 @@
       <c r="B57" s="92"/>
       <c r="C57" s="92"/>
       <c r="D57" s="94"/>
-      <c r="E57" s="199" t="s">
+      <c r="E57" s="204" t="s">
         <v>147</v>
       </c>
-      <c r="F57" s="200"/>
-      <c r="G57" s="200"/>
-      <c r="H57" s="200"/>
-      <c r="I57" s="200"/>
-      <c r="J57" s="200"/>
-      <c r="K57" s="200"/>
-      <c r="L57" s="200"/>
-      <c r="M57" s="200"/>
-      <c r="N57" s="200"/>
-      <c r="O57" s="200"/>
-      <c r="P57" s="200"/>
-      <c r="Q57" s="200"/>
-      <c r="R57" s="200"/>
+      <c r="F57" s="205"/>
+      <c r="G57" s="205"/>
+      <c r="H57" s="205"/>
+      <c r="I57" s="205"/>
+      <c r="J57" s="205"/>
+      <c r="K57" s="205"/>
+      <c r="L57" s="205"/>
+      <c r="M57" s="205"/>
+      <c r="N57" s="205"/>
+      <c r="O57" s="205"/>
+      <c r="P57" s="205"/>
+      <c r="Q57" s="205"/>
+      <c r="R57" s="205"/>
     </row>
     <row r="58" spans="1:18" s="67" customFormat="1" ht="17" customHeight="1">
       <c r="A58" s="107"/>
@@ -10960,22 +11044,22 @@
       <c r="B61" s="66"/>
       <c r="C61" s="66"/>
       <c r="D61" s="71"/>
-      <c r="E61" s="197" t="s">
+      <c r="E61" s="202" t="s">
         <v>178</v>
       </c>
-      <c r="F61" s="198"/>
-      <c r="G61" s="198"/>
-      <c r="H61" s="198"/>
-      <c r="I61" s="198"/>
-      <c r="J61" s="198"/>
-      <c r="K61" s="198"/>
-      <c r="L61" s="198"/>
-      <c r="M61" s="198"/>
-      <c r="N61" s="198"/>
-      <c r="O61" s="198"/>
-      <c r="P61" s="198"/>
-      <c r="Q61" s="198"/>
-      <c r="R61" s="198"/>
+      <c r="F61" s="203"/>
+      <c r="G61" s="203"/>
+      <c r="H61" s="203"/>
+      <c r="I61" s="203"/>
+      <c r="J61" s="203"/>
+      <c r="K61" s="203"/>
+      <c r="L61" s="203"/>
+      <c r="M61" s="203"/>
+      <c r="N61" s="203"/>
+      <c r="O61" s="203"/>
+      <c r="P61" s="203"/>
+      <c r="Q61" s="203"/>
+      <c r="R61" s="203"/>
     </row>
     <row r="62" spans="1:18" s="67" customFormat="1" ht="17" customHeight="1">
       <c r="A62" s="107"/>
@@ -11308,22 +11392,22 @@
       <c r="B77" s="66"/>
       <c r="C77" s="66"/>
       <c r="D77" s="71"/>
-      <c r="E77" s="197" t="s">
+      <c r="E77" s="202" t="s">
         <v>179</v>
       </c>
-      <c r="F77" s="198"/>
-      <c r="G77" s="198"/>
-      <c r="H77" s="198"/>
-      <c r="I77" s="198"/>
-      <c r="J77" s="198"/>
-      <c r="K77" s="198"/>
-      <c r="L77" s="198"/>
-      <c r="M77" s="198"/>
-      <c r="N77" s="198"/>
-      <c r="O77" s="198"/>
-      <c r="P77" s="198"/>
-      <c r="Q77" s="198"/>
-      <c r="R77" s="198"/>
+      <c r="F77" s="203"/>
+      <c r="G77" s="203"/>
+      <c r="H77" s="203"/>
+      <c r="I77" s="203"/>
+      <c r="J77" s="203"/>
+      <c r="K77" s="203"/>
+      <c r="L77" s="203"/>
+      <c r="M77" s="203"/>
+      <c r="N77" s="203"/>
+      <c r="O77" s="203"/>
+      <c r="P77" s="203"/>
+      <c r="Q77" s="203"/>
+      <c r="R77" s="203"/>
     </row>
     <row r="78" spans="1:18" s="67" customFormat="1" ht="13" customHeight="1">
       <c r="A78" s="107"/>
@@ -11350,22 +11434,22 @@
       <c r="B79" s="66"/>
       <c r="C79" s="66"/>
       <c r="D79" s="71"/>
-      <c r="E79" s="197" t="s">
+      <c r="E79" s="202" t="s">
         <v>180</v>
       </c>
-      <c r="F79" s="198"/>
-      <c r="G79" s="198"/>
-      <c r="H79" s="198"/>
-      <c r="I79" s="198"/>
-      <c r="J79" s="198"/>
-      <c r="K79" s="198"/>
-      <c r="L79" s="198"/>
-      <c r="M79" s="198"/>
-      <c r="N79" s="198"/>
-      <c r="O79" s="198"/>
-      <c r="P79" s="198"/>
-      <c r="Q79" s="198"/>
-      <c r="R79" s="198"/>
+      <c r="F79" s="203"/>
+      <c r="G79" s="203"/>
+      <c r="H79" s="203"/>
+      <c r="I79" s="203"/>
+      <c r="J79" s="203"/>
+      <c r="K79" s="203"/>
+      <c r="L79" s="203"/>
+      <c r="M79" s="203"/>
+      <c r="N79" s="203"/>
+      <c r="O79" s="203"/>
+      <c r="P79" s="203"/>
+      <c r="Q79" s="203"/>
+      <c r="R79" s="203"/>
     </row>
     <row r="80" spans="1:18" s="67" customFormat="1" ht="13" customHeight="1">
       <c r="A80" s="107"/>
@@ -11392,22 +11476,22 @@
       <c r="B81" s="66"/>
       <c r="C81" s="66"/>
       <c r="D81" s="71"/>
-      <c r="E81" s="197" t="s">
+      <c r="E81" s="202" t="s">
         <v>181</v>
       </c>
-      <c r="F81" s="198"/>
-      <c r="G81" s="198"/>
-      <c r="H81" s="198"/>
-      <c r="I81" s="198"/>
-      <c r="J81" s="198"/>
-      <c r="K81" s="198"/>
-      <c r="L81" s="198"/>
-      <c r="M81" s="198"/>
-      <c r="N81" s="198"/>
-      <c r="O81" s="198"/>
-      <c r="P81" s="198"/>
-      <c r="Q81" s="198"/>
-      <c r="R81" s="198"/>
+      <c r="F81" s="203"/>
+      <c r="G81" s="203"/>
+      <c r="H81" s="203"/>
+      <c r="I81" s="203"/>
+      <c r="J81" s="203"/>
+      <c r="K81" s="203"/>
+      <c r="L81" s="203"/>
+      <c r="M81" s="203"/>
+      <c r="N81" s="203"/>
+      <c r="O81" s="203"/>
+      <c r="P81" s="203"/>
+      <c r="Q81" s="203"/>
+      <c r="R81" s="203"/>
     </row>
     <row r="82" spans="1:18" s="67" customFormat="1" ht="13" customHeight="1">
       <c r="A82" s="107"/>
@@ -11434,22 +11518,22 @@
       <c r="B83" s="66"/>
       <c r="C83" s="66"/>
       <c r="D83" s="71"/>
-      <c r="E83" s="197" t="s">
+      <c r="E83" s="202" t="s">
         <v>182</v>
       </c>
-      <c r="F83" s="198"/>
-      <c r="G83" s="198"/>
-      <c r="H83" s="198"/>
-      <c r="I83" s="198"/>
-      <c r="J83" s="198"/>
-      <c r="K83" s="198"/>
-      <c r="L83" s="198"/>
-      <c r="M83" s="198"/>
-      <c r="N83" s="198"/>
-      <c r="O83" s="198"/>
-      <c r="P83" s="198"/>
-      <c r="Q83" s="198"/>
-      <c r="R83" s="198"/>
+      <c r="F83" s="203"/>
+      <c r="G83" s="203"/>
+      <c r="H83" s="203"/>
+      <c r="I83" s="203"/>
+      <c r="J83" s="203"/>
+      <c r="K83" s="203"/>
+      <c r="L83" s="203"/>
+      <c r="M83" s="203"/>
+      <c r="N83" s="203"/>
+      <c r="O83" s="203"/>
+      <c r="P83" s="203"/>
+      <c r="Q83" s="203"/>
+      <c r="R83" s="203"/>
     </row>
     <row r="84" spans="1:18" s="67" customFormat="1" ht="13" customHeight="1">
       <c r="A84" s="107"/>
@@ -11476,22 +11560,22 @@
       <c r="B85" s="66"/>
       <c r="C85" s="66"/>
       <c r="D85" s="71"/>
-      <c r="E85" s="197" t="s">
+      <c r="E85" s="202" t="s">
         <v>183</v>
       </c>
-      <c r="F85" s="198"/>
-      <c r="G85" s="198"/>
-      <c r="H85" s="198"/>
-      <c r="I85" s="198"/>
-      <c r="J85" s="198"/>
-      <c r="K85" s="198"/>
-      <c r="L85" s="198"/>
-      <c r="M85" s="198"/>
-      <c r="N85" s="198"/>
-      <c r="O85" s="198"/>
-      <c r="P85" s="198"/>
-      <c r="Q85" s="198"/>
-      <c r="R85" s="198"/>
+      <c r="F85" s="203"/>
+      <c r="G85" s="203"/>
+      <c r="H85" s="203"/>
+      <c r="I85" s="203"/>
+      <c r="J85" s="203"/>
+      <c r="K85" s="203"/>
+      <c r="L85" s="203"/>
+      <c r="M85" s="203"/>
+      <c r="N85" s="203"/>
+      <c r="O85" s="203"/>
+      <c r="P85" s="203"/>
+      <c r="Q85" s="203"/>
+      <c r="R85" s="203"/>
     </row>
     <row r="86" spans="1:18" s="67" customFormat="1" ht="13" customHeight="1">
       <c r="A86" s="107"/>
@@ -11518,22 +11602,22 @@
       <c r="B87" s="66"/>
       <c r="C87" s="66"/>
       <c r="D87" s="71"/>
-      <c r="E87" s="197" t="s">
+      <c r="E87" s="202" t="s">
         <v>184</v>
       </c>
-      <c r="F87" s="198"/>
-      <c r="G87" s="198"/>
-      <c r="H87" s="198"/>
-      <c r="I87" s="198"/>
-      <c r="J87" s="198"/>
-      <c r="K87" s="198"/>
-      <c r="L87" s="198"/>
-      <c r="M87" s="198"/>
-      <c r="N87" s="198"/>
-      <c r="O87" s="198"/>
-      <c r="P87" s="198"/>
-      <c r="Q87" s="198"/>
-      <c r="R87" s="198"/>
+      <c r="F87" s="203"/>
+      <c r="G87" s="203"/>
+      <c r="H87" s="203"/>
+      <c r="I87" s="203"/>
+      <c r="J87" s="203"/>
+      <c r="K87" s="203"/>
+      <c r="L87" s="203"/>
+      <c r="M87" s="203"/>
+      <c r="N87" s="203"/>
+      <c r="O87" s="203"/>
+      <c r="P87" s="203"/>
+      <c r="Q87" s="203"/>
+      <c r="R87" s="203"/>
     </row>
     <row r="88" spans="1:18" s="67" customFormat="1" ht="13" customHeight="1">
       <c r="A88" s="107"/>
@@ -11560,22 +11644,22 @@
       <c r="B89" s="66"/>
       <c r="C89" s="66"/>
       <c r="D89" s="71"/>
-      <c r="E89" s="197" t="s">
+      <c r="E89" s="202" t="s">
         <v>185</v>
       </c>
-      <c r="F89" s="198"/>
-      <c r="G89" s="198"/>
-      <c r="H89" s="198"/>
-      <c r="I89" s="198"/>
-      <c r="J89" s="198"/>
-      <c r="K89" s="198"/>
-      <c r="L89" s="198"/>
-      <c r="M89" s="198"/>
-      <c r="N89" s="198"/>
-      <c r="O89" s="198"/>
-      <c r="P89" s="198"/>
-      <c r="Q89" s="198"/>
-      <c r="R89" s="198"/>
+      <c r="F89" s="203"/>
+      <c r="G89" s="203"/>
+      <c r="H89" s="203"/>
+      <c r="I89" s="203"/>
+      <c r="J89" s="203"/>
+      <c r="K89" s="203"/>
+      <c r="L89" s="203"/>
+      <c r="M89" s="203"/>
+      <c r="N89" s="203"/>
+      <c r="O89" s="203"/>
+      <c r="P89" s="203"/>
+      <c r="Q89" s="203"/>
+      <c r="R89" s="203"/>
     </row>
     <row r="90" spans="1:18" s="67" customFormat="1" ht="17" customHeight="1">
       <c r="A90" s="107"/>
@@ -12475,6 +12559,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E89:R89"/>
+    <mergeCell ref="E77:R77"/>
+    <mergeCell ref="E79:R79"/>
+    <mergeCell ref="E81:R81"/>
+    <mergeCell ref="E83:R83"/>
+    <mergeCell ref="E85:R85"/>
+    <mergeCell ref="E87:R87"/>
     <mergeCell ref="E61:R61"/>
     <mergeCell ref="E19:R19"/>
     <mergeCell ref="E17:R17"/>
@@ -12486,13 +12577,6 @@
     <mergeCell ref="E47:F47"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="E57:R57"/>
-    <mergeCell ref="E89:R89"/>
-    <mergeCell ref="E77:R77"/>
-    <mergeCell ref="E79:R79"/>
-    <mergeCell ref="E81:R81"/>
-    <mergeCell ref="E83:R83"/>
-    <mergeCell ref="E85:R85"/>
-    <mergeCell ref="E87:R87"/>
   </mergeCells>
   <phoneticPr fontId="34" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -12523,17 +12607,17 @@
   <sheetData>
     <row r="33" spans="3:3">
       <c r="C33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="3:3">
       <c r="C34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="35" spans="3:3">
       <c r="C35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>